<commit_message>
Changes in add skill
</commit_message>
<xml_diff>
--- a/MarsFramework/ExcelData/TestData.xlsx
+++ b/MarsFramework/ExcelData/TestData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21727"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21901"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\minty\OneDrive\Documents\Standard\MarsFramework\MarsFramework\ExcelData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="44" documentId="11_40C60FA8E86F796FAE462368AF49F5876813FE7B" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{EA30952A-82D2-4FA4-881B-C83C9FFE555C}"/>
+  <xr:revisionPtr revIDLastSave="90" documentId="11_40C60FA8E86F796FAE462368AF49F5876813FE7B" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{D58EA91C-32F4-4DA7-885C-DD312B8A86EF}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SignUp" sheetId="3" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="56">
   <si>
     <t>Url</t>
   </si>
@@ -165,6 +165,33 @@
   </si>
   <si>
     <t>8152019'</t>
+  </si>
+  <si>
+    <t>On-site</t>
+  </si>
+  <si>
+    <t>Service Type</t>
+  </si>
+  <si>
+    <t>Location</t>
+  </si>
+  <si>
+    <t>Hidden</t>
+  </si>
+  <si>
+    <t>One-off service</t>
+  </si>
+  <si>
+    <t>WorkSamples</t>
+  </si>
+  <si>
+    <t>Music &amp; Audio</t>
+  </si>
+  <si>
+    <t>C:\Users\minty\OneDrive\Documents\Standard\SampleImage.jpg</t>
+  </si>
+  <si>
+    <t>IsActive</t>
   </si>
 </sst>
 </file>
@@ -224,7 +251,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
@@ -235,6 +262,7 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -635,8 +663,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{718D1C37-A02C-4A14-BD8D-CEB2800015BA}">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -708,25 +736,30 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD498EB9-FDAB-43BF-9B49-7521AD3B072F}">
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:M2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="M1" sqref="M1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="24.36328125" customWidth="1"/>
-    <col min="2" max="2" width="27.36328125" customWidth="1"/>
-    <col min="3" max="3" width="20.90625" customWidth="1"/>
-    <col min="4" max="4" width="19.90625" customWidth="1"/>
-    <col min="5" max="5" width="10.26953125" customWidth="1"/>
-    <col min="6" max="6" width="12.08984375" customWidth="1"/>
-    <col min="7" max="7" width="17.7265625" customWidth="1"/>
-    <col min="9" max="9" width="11.90625" customWidth="1"/>
+    <col min="1" max="1" width="16" customWidth="1"/>
+    <col min="2" max="2" width="23.90625" customWidth="1"/>
+    <col min="3" max="3" width="18.1796875" customWidth="1"/>
+    <col min="4" max="4" width="13.26953125" customWidth="1"/>
+    <col min="5" max="5" width="10.6328125" customWidth="1"/>
+    <col min="6" max="6" width="18.7265625" customWidth="1"/>
+    <col min="7" max="7" width="14.7265625" customWidth="1"/>
+    <col min="8" max="8" width="12.08984375" customWidth="1"/>
+    <col min="9" max="9" width="17.7265625" customWidth="1"/>
+    <col min="10" max="10" width="15" customWidth="1"/>
+    <col min="11" max="11" width="10.26953125" customWidth="1"/>
+    <col min="12" max="12" width="27.7265625" customWidth="1"/>
+    <col min="13" max="13" width="19.90625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="17.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:13" s="3" customFormat="1" ht="35" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>32</v>
       </c>
@@ -734,28 +767,40 @@
         <v>15</v>
       </c>
       <c r="C1" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="E1" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="F1" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="J1" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="K1" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="F1" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="H1" t="s">
-        <v>43</v>
-      </c>
-      <c r="I1" t="s">
-        <v>44</v>
+      <c r="L1" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>55</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="58" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:13" ht="29" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>36</v>
       </c>
@@ -763,29 +808,42 @@
         <v>37</v>
       </c>
       <c r="C2" t="s">
+        <v>53</v>
+      </c>
+      <c r="D2">
+        <v>2</v>
+      </c>
+      <c r="E2" t="s">
         <v>38</v>
       </c>
-      <c r="D2" t="s">
+      <c r="F2" t="s">
+        <v>51</v>
+      </c>
+      <c r="G2" t="s">
+        <v>47</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="J2" t="s">
         <v>39</v>
       </c>
-      <c r="E2">
+      <c r="K2">
         <v>10</v>
       </c>
-      <c r="F2" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="G2" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="H2">
-        <v>3</v>
-      </c>
-      <c r="I2">
-        <v>2</v>
+      <c r="L2" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="M2" t="s">
+        <v>50</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -794,7 +852,7 @@
   <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
xpath and wait changes
</commit_message>
<xml_diff>
--- a/MarsFramework/ExcelData/TestData.xlsx
+++ b/MarsFramework/ExcelData/TestData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\minty\OneDrive\Documents\Standard\MarsFramework\MarsFramework\ExcelData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="90" documentId="11_40C60FA8E86F796FAE462368AF49F5876813FE7B" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{D58EA91C-32F4-4DA7-885C-DD312B8A86EF}"/>
+  <xr:revisionPtr revIDLastSave="94" documentId="11_40C60FA8E86F796FAE462368AF49F5876813FE7B" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{AE4FBEB3-6C20-4E0B-9A2C-F62E6A7DAA07}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="58">
   <si>
     <t>Url</t>
   </si>
@@ -192,6 +192,12 @@
   </si>
   <si>
     <t>IsActive</t>
+  </si>
+  <si>
+    <t>Skill Trade</t>
+  </si>
+  <si>
+    <t>Skill-exchange</t>
   </si>
 </sst>
 </file>
@@ -736,10 +742,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD498EB9-FDAB-43BF-9B49-7521AD3B072F}">
-  <dimension ref="A1:M2"/>
+  <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="M1" sqref="M1"/>
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -752,14 +758,15 @@
     <col min="6" max="6" width="18.7265625" customWidth="1"/>
     <col min="7" max="7" width="14.7265625" customWidth="1"/>
     <col min="8" max="8" width="12.08984375" customWidth="1"/>
-    <col min="9" max="9" width="17.7265625" customWidth="1"/>
-    <col min="10" max="10" width="15" customWidth="1"/>
-    <col min="11" max="11" width="10.26953125" customWidth="1"/>
-    <col min="12" max="12" width="27.7265625" customWidth="1"/>
-    <col min="13" max="13" width="19.90625" customWidth="1"/>
+    <col min="9" max="10" width="17.7265625" customWidth="1"/>
+    <col min="11" max="11" width="15" customWidth="1"/>
+    <col min="12" max="12" width="10.26953125" customWidth="1"/>
+    <col min="13" max="13" width="27.7265625" customWidth="1"/>
+    <col min="14" max="14" width="19.90625" customWidth="1"/>
+    <col min="15" max="15" width="18.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="3" customFormat="1" ht="35" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:14" s="3" customFormat="1" ht="35" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>32</v>
       </c>
@@ -788,19 +795,22 @@
         <v>42</v>
       </c>
       <c r="J1" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="K1" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="L1" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="M1" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="M1" s="3" t="s">
+      <c r="N1" s="3" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="29" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:14" ht="29" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>36</v>
       </c>
@@ -828,16 +838,19 @@
       <c r="I2" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="J2" t="s">
+      <c r="J2" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="K2" t="s">
         <v>39</v>
       </c>
-      <c r="K2">
+      <c r="L2">
         <v>10</v>
       </c>
-      <c r="L2" s="6" t="s">
+      <c r="M2" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="M2" t="s">
+      <c r="N2" t="s">
         <v>50</v>
       </c>
     </row>

</xml_diff>